<commit_message>
add changes about encrypt-decrypt
</commit_message>
<xml_diff>
--- a/assets/excel/Book1.xlsx
+++ b/assets/excel/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafli.putra/Documents/Personal/side-hustle/fiverr/automation-test/assets/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B04618-2A3B-CD40-A938-3B48AB63BFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA509EB-F82D-B644-918D-09A6FD58CED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15880" xr2:uid="{B2E14505-B231-014A-9EC1-EF6AED3985A3}"/>
   </bookViews>
@@ -46,15 +46,9 @@
     <t>mercedez@mailinator.com</t>
   </si>
   <si>
-    <t>P@ssword123</t>
-  </si>
-  <si>
     <t>mercede@mailinator.com</t>
   </si>
   <si>
-    <t>P@ssword1234567890</t>
-  </si>
-  <si>
     <t>summary</t>
   </si>
   <si>
@@ -65,6 +59,12 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>UEBzc3dvcmQxMjM=</t>
+  </si>
+  <si>
+    <t>UEBzc3dvcmQxMjM0NTY3ODkw</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,10 +441,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -458,13 +458,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -472,21 +472,21 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{D97B0AEC-4F14-874A-9D27-8ECA26B82E91}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{1D35CC6C-423E-D146-920F-FEC3B27B3E8C}"/>
+    <hyperlink ref="D2" r:id="rId2" display="P@ssword123" xr:uid="{1D35CC6C-423E-D146-920F-FEC3B27B3E8C}"/>
     <hyperlink ref="C3" r:id="rId3" xr:uid="{BD10A2CB-CBAC-CF41-BB93-B4983FE17E5A}"/>
-    <hyperlink ref="D3" r:id="rId4" xr:uid="{5E0668B1-277D-FA49-BE1C-60CDA06D961E}"/>
+    <hyperlink ref="D3" r:id="rId4" display="P@ssword1234567890" xr:uid="{5E0668B1-277D-FA49-BE1C-60CDA06D961E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added dynamic value test cases
</commit_message>
<xml_diff>
--- a/assets/excel/Book1.xlsx
+++ b/assets/excel/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafli.putra/Documents/Personal/side-hustle/fiverr/automation-test/assets/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA509EB-F82D-B644-918D-09A6FD58CED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673F88A6-1E2A-8F41-955C-346F8AEEBC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15880" xr2:uid="{B2E14505-B231-014A-9EC1-EF6AED3985A3}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>